<commit_message>
Add additional budget documents
</commit_message>
<xml_diff>
--- a/budget/TERN_KI_India_Y1+2+3_Budget_29082025.xlsx
+++ b/budget/TERN_KI_India_Y1+2+3_Budget_29082025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abassi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/Documents/advance-trauma-trial/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59F305F-D063-4A57-8F62-F53AE86B5736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18D1E91-253E-C740-B8C4-100AA69E33E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TERN_KI Budget_190724" sheetId="2" r:id="rId1"/>
@@ -251,9 +251,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * \-??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * \-??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -370,7 +370,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
@@ -378,8 +378,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -394,16 +394,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -415,15 +415,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -451,16 +451,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -792,21 +792,21 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.21875" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.21875" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -820,7 +820,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -844,7 +844,7 @@
       </c>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -873,7 +873,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -902,7 +902,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -931,7 +931,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -960,7 +960,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -989,7 +989,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>9</v>
       </c>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>10</v>
       </c>
@@ -1052,7 +1052,7 @@
       <c r="H10" s="16"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>1</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>2</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>3</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
         <v>15</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
         <v>16</v>
       </c>
@@ -1195,7 +1195,7 @@
       <c r="G16" s="11"/>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>2</v>
       </c>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>1</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>2</v>
       </c>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="H19" s="16"/>
     </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>20</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
         <v>21</v>
       </c>
@@ -1306,7 +1306,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="16"/>
     </row>
-    <row r="22" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>1</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>2</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
         <v>25</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
         <v>26</v>
       </c>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
         <v>31</v>
       </c>
@@ -1447,13 +1447,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="16"/>
     </row>
-    <row r="29" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1461,17 +1461,17 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I31" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I32" t="s">
         <v>46</v>
       </c>
@@ -1501,25 +1501,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62375E20-B086-4152-9E9F-7A135CE43396}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.21875" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>9</v>
       </c>
@@ -1772,7 +1772,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="34" t="s">
         <v>10</v>
       </c>
@@ -1785,7 +1785,7 @@
       <c r="H11" s="19"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>1</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>2</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>3</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>4</v>
       </c>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>5</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>6</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>7</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>8</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>9</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>10</v>
       </c>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>11</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
         <v>15</v>
       </c>
@@ -2131,7 +2131,7 @@
       </c>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
         <v>16</v>
       </c>
@@ -2143,7 +2143,7 @@
       <c r="G25" s="11"/>
       <c r="H25" s="12"/>
     </row>
-    <row r="26" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>2</v>
       </c>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="H26" s="12"/>
     </row>
-    <row r="27" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>1</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>2</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
         <v>20</v>
       </c>
@@ -2241,7 +2241,7 @@
       </c>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
         <v>21</v>
       </c>
@@ -2253,7 +2253,7 @@
       <c r="G30" s="14"/>
       <c r="H30" s="19"/>
     </row>
-    <row r="31" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="H31" s="19"/>
     </row>
-    <row r="32" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="12">
         <v>1</v>
       </c>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="I32" s="18"/>
     </row>
-    <row r="33" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>2</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
         <v>25</v>
       </c>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="H34" s="19"/>
     </row>
-    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
         <v>26</v>
       </c>
@@ -2374,7 +2374,7 @@
       </c>
       <c r="I35" s="17"/>
     </row>
-    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
         <v>68</v>
       </c>
@@ -2386,21 +2386,24 @@
       <c r="G36" s="5"/>
       <c r="H36" s="19"/>
     </row>
-    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="16"/>
     </row>
-    <row r="38" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G38" s="2">
+        <f>G35/2*1.25</f>
+        <v>2822050.561797753</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>

</xml_diff>